<commit_message>
Test cartpole v1 completed
</commit_message>
<xml_diff>
--- a/Tests_v1.xlsx
+++ b/Tests_v1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X63"/>
+  <dimension ref="A1:Y62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -554,6 +554,11 @@
           <t>Total Runtime</t>
         </is>
       </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Error Message</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -636,6 +641,7 @@
       <c r="X2" t="n">
         <v>12.7610991001129</v>
       </c>
+      <c r="Y2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -718,6 +724,7 @@
       <c r="X3" t="n">
         <v>103.373969078063</v>
       </c>
+      <c r="Y3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -800,6 +807,7 @@
       <c r="X4" t="n">
         <v>25.9728763103485</v>
       </c>
+      <c r="Y4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -882,6 +890,7 @@
       <c r="X5" t="n">
         <v>104.556809425354</v>
       </c>
+      <c r="Y5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -964,6 +973,7 @@
       <c r="X6" t="n">
         <v>707.314825773239</v>
       </c>
+      <c r="Y6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -1046,6 +1056,7 @@
       <c r="X7" t="n">
         <v>298.112325191497</v>
       </c>
+      <c r="Y7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1128,6 +1139,7 @@
       <c r="X8" t="n">
         <v>834.02043390274</v>
       </c>
+      <c r="Y8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1210,6 +1222,7 @@
       <c r="X9" t="n">
         <v>170.661868095397</v>
       </c>
+      <c r="Y9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1292,6 +1305,7 @@
       <c r="X10" t="n">
         <v>360.051567792892</v>
       </c>
+      <c r="Y10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1374,6 +1388,7 @@
       <c r="X11" t="n">
         <v>342.883033037185</v>
       </c>
+      <c r="Y11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1456,6 +1471,7 @@
       <c r="X12" t="n">
         <v>1490.26040363311</v>
       </c>
+      <c r="Y12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1538,6 +1554,7 @@
       <c r="X13" t="n">
         <v>190.771907567977</v>
       </c>
+      <c r="Y13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1620,6 +1637,7 @@
       <c r="X14" t="n">
         <v>677.255814552307</v>
       </c>
+      <c r="Y14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1702,6 +1720,7 @@
       <c r="X15" t="n">
         <v>549.525586605072</v>
       </c>
+      <c r="Y15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1784,6 +1803,7 @@
       <c r="X16" t="n">
         <v>1801.17230892181</v>
       </c>
+      <c r="Y16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1866,6 +1886,7 @@
       <c r="X17" t="n">
         <v>1021.90316963195</v>
       </c>
+      <c r="Y17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1948,6 +1969,7 @@
       <c r="X18" t="n">
         <v>145.756466865539</v>
       </c>
+      <c r="Y18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -2030,6 +2052,7 @@
       <c r="X19" t="n">
         <v>695.08347916603</v>
       </c>
+      <c r="Y19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -2112,6 +2135,7 @@
       <c r="X20" t="n">
         <v>586.083564043045</v>
       </c>
+      <c r="Y20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -2194,6 +2218,7 @@
       <c r="X21" t="n">
         <v>645.909253120422</v>
       </c>
+      <c r="Y21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -2276,6 +2301,7 @@
       <c r="X22" t="n">
         <v>638.266948223114</v>
       </c>
+      <c r="Y22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -2358,6 +2384,7 @@
       <c r="X23" t="n">
         <v>666.6037654876709</v>
       </c>
+      <c r="Y23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -2440,6 +2467,7 @@
       <c r="X24" t="n">
         <v>1500.047805786133</v>
       </c>
+      <c r="Y24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -2522,6 +2550,7 @@
       <c r="X25" t="n">
         <v>442.0760726928711</v>
       </c>
+      <c r="Y25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -2604,6 +2633,7 @@
       <c r="X26" t="n">
         <v>1281.828253507614</v>
       </c>
+      <c r="Y26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -2686,6 +2716,7 @@
       <c r="X27" t="n">
         <v>1117.778146982193</v>
       </c>
+      <c r="Y27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -2768,6 +2799,7 @@
       <c r="X28" t="n">
         <v>497.579952955246</v>
       </c>
+      <c r="Y28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2850,6 +2882,7 @@
       <c r="X29" t="n">
         <v>722.5147490501404</v>
       </c>
+      <c r="Y29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -2932,6 +2965,7 @@
       <c r="X30" t="n">
         <v>1494.248463869095</v>
       </c>
+      <c r="Y30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -3014,6 +3048,7 @@
       <c r="X31" t="n">
         <v>570.1489367485046</v>
       </c>
+      <c r="Y31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -3096,6 +3131,7 @@
       <c r="X32" t="n">
         <v>386.126457452774</v>
       </c>
+      <c r="Y32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -3178,6 +3214,7 @@
       <c r="X33" t="n">
         <v>1335.486039400101</v>
       </c>
+      <c r="Y33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -3260,6 +3297,7 @@
       <c r="X34" t="n">
         <v>502.3282358646393</v>
       </c>
+      <c r="Y34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -3342,6 +3380,7 @@
       <c r="X35" t="n">
         <v>1419.859392881393</v>
       </c>
+      <c r="Y35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -3424,6 +3463,7 @@
       <c r="X36" t="n">
         <v>2026.390106678009</v>
       </c>
+      <c r="Y36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -3506,6 +3546,7 @@
       <c r="X37" t="n">
         <v>1728.064740419388</v>
       </c>
+      <c r="Y37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -3529,13 +3570,11 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>BEST OF ABOVE</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>BEST OF ABOVE</t>
-        </is>
+          <t>inversion</t>
+        </is>
+      </c>
+      <c r="G38" t="n">
+        <v>0.2</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
@@ -3543,7 +3582,7 @@
         </is>
       </c>
       <c r="I38" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -3569,19 +3608,28 @@
       </c>
       <c r="P38" t="inlineStr"/>
       <c r="Q38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R38" t="inlineStr"/>
       <c r="S38" t="inlineStr">
         <is>
-          <t>Elitism selection, agents = 2</t>
+          <t>Elitism selection, agents = 5</t>
         </is>
       </c>
       <c r="T38" t="inlineStr"/>
-      <c r="U38" t="inlineStr"/>
-      <c r="V38" t="inlineStr"/>
-      <c r="W38" t="inlineStr"/>
-      <c r="X38" t="inlineStr"/>
+      <c r="U38" t="n">
+        <v>68</v>
+      </c>
+      <c r="V38" t="n">
+        <v>250</v>
+      </c>
+      <c r="W38" t="n">
+        <v>45.3011817574501</v>
+      </c>
+      <c r="X38" t="n">
+        <v>906.0236351490021</v>
+      </c>
+      <c r="Y38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -3605,13 +3653,11 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>inversion</t>
+        </is>
+      </c>
+      <c r="G39" t="n">
+        <v>0.2</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
@@ -3619,7 +3665,7 @@
         </is>
       </c>
       <c r="I39" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -3645,19 +3691,28 @@
       </c>
       <c r="P39" t="inlineStr"/>
       <c r="Q39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R39" t="inlineStr"/>
       <c r="S39" t="inlineStr">
         <is>
-          <t>Elitism selection, agents = 5</t>
+          <t>Elitism selection, agents = 10</t>
         </is>
       </c>
       <c r="T39" t="inlineStr"/>
-      <c r="U39" t="inlineStr"/>
-      <c r="V39" t="inlineStr"/>
-      <c r="W39" t="inlineStr"/>
-      <c r="X39" t="inlineStr"/>
+      <c r="U39" t="n">
+        <v>139</v>
+      </c>
+      <c r="V39" t="n">
+        <v>250</v>
+      </c>
+      <c r="W39" t="n">
+        <v>83.6733537554741</v>
+      </c>
+      <c r="X39" t="n">
+        <v>1673.467075109482</v>
+      </c>
+      <c r="Y39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -3681,21 +3736,19 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>inversion</t>
+        </is>
+      </c>
+      <c r="G40" t="n">
+        <v>0.2</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>elitism</t>
+          <t>tournament</t>
         </is>
       </c>
       <c r="I40" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -3721,19 +3774,28 @@
       </c>
       <c r="P40" t="inlineStr"/>
       <c r="Q40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R40" t="inlineStr"/>
       <c r="S40" t="inlineStr">
         <is>
-          <t>Elitism selection, agents = 10</t>
+          <t>tournament selection, agents = 2</t>
         </is>
       </c>
       <c r="T40" t="inlineStr"/>
-      <c r="U40" t="inlineStr"/>
-      <c r="V40" t="inlineStr"/>
-      <c r="W40" t="inlineStr"/>
-      <c r="X40" t="inlineStr"/>
+      <c r="U40" t="n">
+        <v>9</v>
+      </c>
+      <c r="V40" t="n">
+        <v>86</v>
+      </c>
+      <c r="W40" t="n">
+        <v>18.2298110961914</v>
+      </c>
+      <c r="X40" t="n">
+        <v>364.5962219238281</v>
+      </c>
+      <c r="Y40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -3757,13 +3819,11 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>inversion</t>
+        </is>
+      </c>
+      <c r="G41" t="n">
+        <v>0.2</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
@@ -3771,7 +3831,7 @@
         </is>
       </c>
       <c r="I41" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -3797,19 +3857,28 @@
       </c>
       <c r="P41" t="inlineStr"/>
       <c r="Q41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R41" t="inlineStr"/>
       <c r="S41" t="inlineStr">
         <is>
-          <t>tournament selection, agents = 2</t>
+          <t>tournament selection, agents = 5</t>
         </is>
       </c>
       <c r="T41" t="inlineStr"/>
-      <c r="U41" t="inlineStr"/>
-      <c r="V41" t="inlineStr"/>
-      <c r="W41" t="inlineStr"/>
-      <c r="X41" t="inlineStr"/>
+      <c r="U41" t="n">
+        <v>24</v>
+      </c>
+      <c r="V41" t="n">
+        <v>250</v>
+      </c>
+      <c r="W41" t="n">
+        <v>19.47060992717743</v>
+      </c>
+      <c r="X41" t="n">
+        <v>389.4121985435486</v>
+      </c>
+      <c r="Y41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -3833,13 +3902,11 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>inversion</t>
+        </is>
+      </c>
+      <c r="G42" t="n">
+        <v>0.2</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
@@ -3847,7 +3914,7 @@
         </is>
       </c>
       <c r="I42" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -3878,14 +3945,36 @@
       <c r="R42" t="inlineStr"/>
       <c r="S42" t="inlineStr">
         <is>
-          <t>tournament selection, agents = 5</t>
+          <t>tournament selection, agents = 10</t>
         </is>
       </c>
       <c r="T42" t="inlineStr"/>
-      <c r="U42" t="inlineStr"/>
-      <c r="V42" t="inlineStr"/>
-      <c r="W42" t="inlineStr"/>
-      <c r="X42" t="inlineStr"/>
+      <c r="U42" t="n">
+        <v>0</v>
+      </c>
+      <c r="V42" t="n">
+        <v>0</v>
+      </c>
+      <c r="W42" t="n">
+        <v>0</v>
+      </c>
+      <c r="X42" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Traceback (most recent call last):
+  File "C:\Users\aasav\github-classroom\EMAT31530\group-project-2\automated_testing.py", line 103, in &lt;module&gt;
+    ga.run()
+  File "C:\Users\aasav\github-classroom\EMAT31530\group-project-2\GeneticAlgorithm.py", line 153, in run
+    self = selection(self)
+  File "C:\Users\aasav\github-classroom\EMAT31530\group-project-2\selection.py", line 58, in selection
+    tournament = np.random.choice(range(len(population)), tournament_size, replace=True)
+  File "mtrand.pyx", line 934, in numpy.random.mtrand.RandomState.choice
+ValueError: 'a' cannot be empty unless no samples are taken
+</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -3909,21 +3998,19 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>inversion</t>
+        </is>
+      </c>
+      <c r="G43" t="n">
+        <v>0.2</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>tournament</t>
+          <t>proportional-roulette-wheel</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -3954,14 +4041,37 @@
       <c r="R43" t="inlineStr"/>
       <c r="S43" t="inlineStr">
         <is>
-          <t>tournament selection, agents = 10</t>
+          <t>proportional-roulette-wheel selection, agents = 2</t>
         </is>
       </c>
       <c r="T43" t="inlineStr"/>
-      <c r="U43" t="inlineStr"/>
-      <c r="V43" t="inlineStr"/>
-      <c r="W43" t="inlineStr"/>
-      <c r="X43" t="inlineStr"/>
+      <c r="U43" t="n">
+        <v>0</v>
+      </c>
+      <c r="V43" t="n">
+        <v>0</v>
+      </c>
+      <c r="W43" t="n">
+        <v>0</v>
+      </c>
+      <c r="X43" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Traceback (most recent call last):
+  File "C:\Users\aasav\github-classroom\EMAT31530\group-project-2\automated_testing.py", line 103, in &lt;module&gt;
+    ga.run()
+  File "C:\Users\aasav\github-classroom\EMAT31530\group-project-2\GeneticAlgorithm.py", line 156, in run
+    self = crossover(self)
+  File "C:\Users\aasav\github-classroom\EMAT31530\group-project-2\crossover.py", line 46, in crossover
+    parent1 = selected_parents[random.choice(range(len(selected_parents)))]
+  File "C:\Users\aasav\miniconda3\envs\ga_env\lib\random.py", line 378, in choice
+    return seq[self._randbelow(len(seq))]
+IndexError: range object index out of range
+</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -3985,13 +4095,11 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>inversion</t>
+        </is>
+      </c>
+      <c r="G44" t="n">
+        <v>0.2</v>
       </c>
       <c r="H44" t="inlineStr">
         <is>
@@ -3999,7 +4107,7 @@
         </is>
       </c>
       <c r="I44" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -4030,14 +4138,37 @@
       <c r="R44" t="inlineStr"/>
       <c r="S44" t="inlineStr">
         <is>
-          <t>proportional-roulette-wheel selection, agents = 2</t>
+          <t>proportional-roulette-wheel selection, agents = 5</t>
         </is>
       </c>
       <c r="T44" t="inlineStr"/>
-      <c r="U44" t="inlineStr"/>
-      <c r="V44" t="inlineStr"/>
-      <c r="W44" t="inlineStr"/>
-      <c r="X44" t="inlineStr"/>
+      <c r="U44" t="n">
+        <v>0</v>
+      </c>
+      <c r="V44" t="n">
+        <v>0</v>
+      </c>
+      <c r="W44" t="n">
+        <v>0</v>
+      </c>
+      <c r="X44" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Traceback (most recent call last):
+  File "C:\Users\aasav\github-classroom\EMAT31530\group-project-2\automated_testing.py", line 103, in &lt;module&gt;
+    ga.run()
+  File "C:\Users\aasav\github-classroom\EMAT31530\group-project-2\GeneticAlgorithm.py", line 156, in run
+    self = crossover(self)
+  File "C:\Users\aasav\github-classroom\EMAT31530\group-project-2\crossover.py", line 46, in crossover
+    parent1 = selected_parents[random.choice(range(len(selected_parents)))]
+  File "C:\Users\aasav\miniconda3\envs\ga_env\lib\random.py", line 378, in choice
+    return seq[self._randbelow(len(seq))]
+IndexError: range object index out of range
+</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -4061,13 +4192,11 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>inversion</t>
+        </is>
+      </c>
+      <c r="G45" t="n">
+        <v>0.2</v>
       </c>
       <c r="H45" t="inlineStr">
         <is>
@@ -4075,7 +4204,7 @@
         </is>
       </c>
       <c r="I45" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -4106,14 +4235,37 @@
       <c r="R45" t="inlineStr"/>
       <c r="S45" t="inlineStr">
         <is>
-          <t>proportional-roulette-wheel selection, agents = 5</t>
+          <t>proportional-roulette-wheel selection, agents = 10</t>
         </is>
       </c>
       <c r="T45" t="inlineStr"/>
-      <c r="U45" t="inlineStr"/>
-      <c r="V45" t="inlineStr"/>
-      <c r="W45" t="inlineStr"/>
-      <c r="X45" t="inlineStr"/>
+      <c r="U45" t="n">
+        <v>0</v>
+      </c>
+      <c r="V45" t="n">
+        <v>0</v>
+      </c>
+      <c r="W45" t="n">
+        <v>0</v>
+      </c>
+      <c r="X45" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Traceback (most recent call last):
+  File "C:\Users\aasav\github-classroom\EMAT31530\group-project-2\automated_testing.py", line 103, in &lt;module&gt;
+    ga.run()
+  File "C:\Users\aasav\github-classroom\EMAT31530\group-project-2\GeneticAlgorithm.py", line 156, in run
+    self = crossover(self)
+  File "C:\Users\aasav\github-classroom\EMAT31530\group-project-2\crossover.py", line 46, in crossover
+    parent1 = selected_parents[random.choice(range(len(selected_parents)))]
+  File "C:\Users\aasav\miniconda3\envs\ga_env\lib\random.py", line 378, in choice
+    return seq[self._randbelow(len(seq))]
+IndexError: range object index out of range
+</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -4137,21 +4289,19 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>inversion</t>
+        </is>
+      </c>
+      <c r="G46" t="n">
+        <v>0.2</v>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>proportional-roulette-wheel</t>
+          <t>rank-based-rolette-wheel</t>
         </is>
       </c>
       <c r="I46" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -4177,19 +4327,28 @@
       </c>
       <c r="P46" t="inlineStr"/>
       <c r="Q46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R46" t="inlineStr"/>
       <c r="S46" t="inlineStr">
         <is>
-          <t>proportional-roulette-wheel selection, agents = 10</t>
+          <t>rank-based-rolette-wheel selection, agents = 2</t>
         </is>
       </c>
       <c r="T46" t="inlineStr"/>
-      <c r="U46" t="inlineStr"/>
-      <c r="V46" t="inlineStr"/>
-      <c r="W46" t="inlineStr"/>
-      <c r="X46" t="inlineStr"/>
+      <c r="U46" t="n">
+        <v>5</v>
+      </c>
+      <c r="V46" t="n">
+        <v>53</v>
+      </c>
+      <c r="W46" t="n">
+        <v>27.19994629621506</v>
+      </c>
+      <c r="X46" t="n">
+        <v>543.9989259243011</v>
+      </c>
+      <c r="Y46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -4213,13 +4372,11 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>inversion</t>
+        </is>
+      </c>
+      <c r="G47" t="n">
+        <v>0.2</v>
       </c>
       <c r="H47" t="inlineStr">
         <is>
@@ -4227,7 +4384,7 @@
         </is>
       </c>
       <c r="I47" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -4253,19 +4410,28 @@
       </c>
       <c r="P47" t="inlineStr"/>
       <c r="Q47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R47" t="inlineStr"/>
       <c r="S47" t="inlineStr">
         <is>
-          <t>rank-based-rolette-wheel selection, agents = 2</t>
+          <t>rank-based-rolette-wheel selection, agents = 5</t>
         </is>
       </c>
       <c r="T47" t="inlineStr"/>
-      <c r="U47" t="inlineStr"/>
-      <c r="V47" t="inlineStr"/>
-      <c r="W47" t="inlineStr"/>
-      <c r="X47" t="inlineStr"/>
+      <c r="U47" t="n">
+        <v>11</v>
+      </c>
+      <c r="V47" t="n">
+        <v>250</v>
+      </c>
+      <c r="W47" t="n">
+        <v>52.38660390377045</v>
+      </c>
+      <c r="X47" t="n">
+        <v>1047.732078075409</v>
+      </c>
+      <c r="Y47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -4289,13 +4455,11 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>inversion</t>
+        </is>
+      </c>
+      <c r="G48" t="n">
+        <v>0.2</v>
       </c>
       <c r="H48" t="inlineStr">
         <is>
@@ -4303,7 +4467,7 @@
         </is>
       </c>
       <c r="I48" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -4329,19 +4493,28 @@
       </c>
       <c r="P48" t="inlineStr"/>
       <c r="Q48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R48" t="inlineStr"/>
       <c r="S48" t="inlineStr">
         <is>
-          <t>rank-based-rolette-wheel selection, agents = 5</t>
+          <t>rank-based-rolette-wheel selection, agents = 10</t>
         </is>
       </c>
       <c r="T48" t="inlineStr"/>
-      <c r="U48" t="inlineStr"/>
-      <c r="V48" t="inlineStr"/>
-      <c r="W48" t="inlineStr"/>
-      <c r="X48" t="inlineStr"/>
+      <c r="U48" t="n">
+        <v>10</v>
+      </c>
+      <c r="V48" t="n">
+        <v>107</v>
+      </c>
+      <c r="W48" t="n">
+        <v>22.35308337211609</v>
+      </c>
+      <c r="X48" t="n">
+        <v>447.0616674423218</v>
+      </c>
+      <c r="Y48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -4365,21 +4538,19 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>inversion</t>
+        </is>
+      </c>
+      <c r="G49" t="n">
+        <v>0.2</v>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>rank-based-rolette-wheel</t>
+          <t>elitism</t>
         </is>
       </c>
       <c r="I49" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -4391,11 +4562,11 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>fixed</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="N49" t="n">
         <v>0</v>
@@ -4405,19 +4576,28 @@
       </c>
       <c r="P49" t="inlineStr"/>
       <c r="Q49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R49" t="inlineStr"/>
       <c r="S49" t="inlineStr">
         <is>
-          <t>rank-based-rolette-wheel selection, agents = 10</t>
+          <t>fixed random agent, rate = 0.1</t>
         </is>
       </c>
       <c r="T49" t="inlineStr"/>
-      <c r="U49" t="inlineStr"/>
-      <c r="V49" t="inlineStr"/>
-      <c r="W49" t="inlineStr"/>
-      <c r="X49" t="inlineStr"/>
+      <c r="U49" t="n">
+        <v>39</v>
+      </c>
+      <c r="V49" t="n">
+        <v>208</v>
+      </c>
+      <c r="W49" t="n">
+        <v>35.94669387340546</v>
+      </c>
+      <c r="X49" t="n">
+        <v>718.9338774681091</v>
+      </c>
+      <c r="Y49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -4441,23 +4621,19 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>inversion</t>
+        </is>
+      </c>
+      <c r="G50" t="n">
+        <v>0.2</v>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>BEST OF ABOVE</t>
-        </is>
-      </c>
-      <c r="I50" t="inlineStr">
-        <is>
-          <t>BEST OF ABOVE</t>
-        </is>
+          <t>elitism</t>
+        </is>
+      </c>
+      <c r="I50" t="n">
+        <v>2</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -4473,7 +4649,7 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="N50" t="n">
         <v>0</v>
@@ -4483,19 +4659,28 @@
       </c>
       <c r="P50" t="inlineStr"/>
       <c r="Q50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R50" t="inlineStr"/>
       <c r="S50" t="inlineStr">
         <is>
-          <t>fixed random agent, rate = 0.1</t>
+          <t>fixed random agent, rate = 0.2</t>
         </is>
       </c>
       <c r="T50" t="inlineStr"/>
-      <c r="U50" t="inlineStr"/>
-      <c r="V50" t="inlineStr"/>
-      <c r="W50" t="inlineStr"/>
-      <c r="X50" t="inlineStr"/>
+      <c r="U50" t="n">
+        <v>41</v>
+      </c>
+      <c r="V50" t="n">
+        <v>250</v>
+      </c>
+      <c r="W50" t="n">
+        <v>39.65939347743988</v>
+      </c>
+      <c r="X50" t="n">
+        <v>793.1878695487976</v>
+      </c>
+      <c r="Y50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -4519,23 +4704,19 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>inversion</t>
+        </is>
+      </c>
+      <c r="G51" t="n">
+        <v>0.2</v>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="I51" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>elitism</t>
+        </is>
+      </c>
+      <c r="I51" t="n">
+        <v>2</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -4551,7 +4732,7 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="N51" t="n">
         <v>0</v>
@@ -4561,19 +4742,28 @@
       </c>
       <c r="P51" t="inlineStr"/>
       <c r="Q51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R51" t="inlineStr"/>
       <c r="S51" t="inlineStr">
         <is>
-          <t>fixed random agent, rate = 0.2</t>
+          <t>fixed random agent, rate = 0.5</t>
         </is>
       </c>
       <c r="T51" t="inlineStr"/>
-      <c r="U51" t="inlineStr"/>
-      <c r="V51" t="inlineStr"/>
-      <c r="W51" t="inlineStr"/>
-      <c r="X51" t="inlineStr"/>
+      <c r="U51" t="n">
+        <v>64</v>
+      </c>
+      <c r="V51" t="n">
+        <v>250</v>
+      </c>
+      <c r="W51" t="n">
+        <v>84.50161932706833</v>
+      </c>
+      <c r="X51" t="n">
+        <v>1690.032386541367</v>
+      </c>
+      <c r="Y51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -4597,23 +4787,19 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>inversion</t>
+        </is>
+      </c>
+      <c r="G52" t="n">
+        <v>0.2</v>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>elitism</t>
+        </is>
+      </c>
+      <c r="I52" t="n">
+        <v>2</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -4625,11 +4811,11 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>fixed</t>
+          <t>linear</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="N52" t="n">
         <v>0</v>
@@ -4644,14 +4830,37 @@
       <c r="R52" t="inlineStr"/>
       <c r="S52" t="inlineStr">
         <is>
-          <t>fixed random agent, rate = 0.5</t>
+          <t>linear random agent, rate = 0.1</t>
         </is>
       </c>
       <c r="T52" t="inlineStr"/>
-      <c r="U52" t="inlineStr"/>
-      <c r="V52" t="inlineStr"/>
-      <c r="W52" t="inlineStr"/>
-      <c r="X52" t="inlineStr"/>
+      <c r="U52" t="n">
+        <v>0</v>
+      </c>
+      <c r="V52" t="n">
+        <v>0</v>
+      </c>
+      <c r="W52" t="n">
+        <v>0</v>
+      </c>
+      <c r="X52" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Traceback (most recent call last):
+  File "C:\Users\aasav\github-classroom\EMAT31530\group-project-2\automated_testing.py", line 103, in &lt;module&gt;
+    ga.run()
+  File "C:\Users\aasav\github-classroom\EMAT31530\group-project-2\GeneticAlgorithm.py", line 162, in run
+    self = random_agent(self)
+  File "C:\Users\aasav\github-classroom\EMAT31530\group-project-2\random_agents.py", line 38, in random_agent
+    random_rate = random_probability(self)
+  File "C:\Users\aasav\github-classroom\EMAT31530\group-project-2\random_agents.py", line 18, in random_probability
+    return random_rate
+UnboundLocalError: local variable 'random_rate' referenced before assignment
+</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -4675,23 +4884,19 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>inversion</t>
+        </is>
+      </c>
+      <c r="G53" t="n">
+        <v>0.2</v>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="I53" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>elitism</t>
+        </is>
+      </c>
+      <c r="I53" t="n">
+        <v>2</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -4707,7 +4912,7 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="N53" t="n">
         <v>0</v>
@@ -4722,14 +4927,37 @@
       <c r="R53" t="inlineStr"/>
       <c r="S53" t="inlineStr">
         <is>
-          <t>linear random agent, rate = 0.1</t>
+          <t>linear random agent, rate = 0.2</t>
         </is>
       </c>
       <c r="T53" t="inlineStr"/>
-      <c r="U53" t="inlineStr"/>
-      <c r="V53" t="inlineStr"/>
-      <c r="W53" t="inlineStr"/>
-      <c r="X53" t="inlineStr"/>
+      <c r="U53" t="n">
+        <v>0</v>
+      </c>
+      <c r="V53" t="n">
+        <v>0</v>
+      </c>
+      <c r="W53" t="n">
+        <v>0</v>
+      </c>
+      <c r="X53" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Traceback (most recent call last):
+  File "C:\Users\aasav\github-classroom\EMAT31530\group-project-2\automated_testing.py", line 103, in &lt;module&gt;
+    ga.run()
+  File "C:\Users\aasav\github-classroom\EMAT31530\group-project-2\GeneticAlgorithm.py", line 162, in run
+    self = random_agent(self)
+  File "C:\Users\aasav\github-classroom\EMAT31530\group-project-2\random_agents.py", line 38, in random_agent
+    random_rate = random_probability(self)
+  File "C:\Users\aasav\github-classroom\EMAT31530\group-project-2\random_agents.py", line 18, in random_probability
+    return random_rate
+UnboundLocalError: local variable 'random_rate' referenced before assignment
+</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -4753,23 +4981,19 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>inversion</t>
+        </is>
+      </c>
+      <c r="G54" t="n">
+        <v>0.2</v>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="I54" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>elitism</t>
+        </is>
+      </c>
+      <c r="I54" t="n">
+        <v>2</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -4785,7 +5009,7 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="N54" t="n">
         <v>0</v>
@@ -4800,14 +5024,37 @@
       <c r="R54" t="inlineStr"/>
       <c r="S54" t="inlineStr">
         <is>
-          <t>linear random agent, rate = 0.2</t>
+          <t>linear random agent, rate = 0.5</t>
         </is>
       </c>
       <c r="T54" t="inlineStr"/>
-      <c r="U54" t="inlineStr"/>
-      <c r="V54" t="inlineStr"/>
-      <c r="W54" t="inlineStr"/>
-      <c r="X54" t="inlineStr"/>
+      <c r="U54" t="n">
+        <v>0</v>
+      </c>
+      <c r="V54" t="n">
+        <v>0</v>
+      </c>
+      <c r="W54" t="n">
+        <v>0</v>
+      </c>
+      <c r="X54" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Traceback (most recent call last):
+  File "C:\Users\aasav\github-classroom\EMAT31530\group-project-2\automated_testing.py", line 103, in &lt;module&gt;
+    ga.run()
+  File "C:\Users\aasav\github-classroom\EMAT31530\group-project-2\GeneticAlgorithm.py", line 162, in run
+    self = random_agent(self)
+  File "C:\Users\aasav\github-classroom\EMAT31530\group-project-2\random_agents.py", line 38, in random_agent
+    random_rate = random_probability(self)
+  File "C:\Users\aasav\github-classroom\EMAT31530\group-project-2\random_agents.py", line 18, in random_probability
+    return random_rate
+UnboundLocalError: local variable 'random_rate' referenced before assignment
+</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -4831,23 +5078,19 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>inversion</t>
+        </is>
+      </c>
+      <c r="G55" t="n">
+        <v>0.2</v>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="I55" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>elitism</t>
+        </is>
+      </c>
+      <c r="I55" t="n">
+        <v>2</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -4859,11 +5102,11 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>linear</t>
+          <t>exponential</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="N55" t="n">
         <v>0</v>
@@ -4873,19 +5116,28 @@
       </c>
       <c r="P55" t="inlineStr"/>
       <c r="Q55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R55" t="inlineStr"/>
       <c r="S55" t="inlineStr">
         <is>
-          <t>linear random agent, rate = 0.5</t>
+          <t>exponential random agent, rate = 0.1</t>
         </is>
       </c>
       <c r="T55" t="inlineStr"/>
-      <c r="U55" t="inlineStr"/>
-      <c r="V55" t="inlineStr"/>
-      <c r="W55" t="inlineStr"/>
-      <c r="X55" t="inlineStr"/>
+      <c r="U55" t="n">
+        <v>102</v>
+      </c>
+      <c r="V55" t="n">
+        <v>250</v>
+      </c>
+      <c r="W55" t="n">
+        <v>65.92817358970642</v>
+      </c>
+      <c r="X55" t="n">
+        <v>1318.563471794128</v>
+      </c>
+      <c r="Y55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -4909,23 +5161,19 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>inversion</t>
+        </is>
+      </c>
+      <c r="G56" t="n">
+        <v>0.2</v>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="I56" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>elitism</t>
+        </is>
+      </c>
+      <c r="I56" t="n">
+        <v>2</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -4941,7 +5189,7 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="N56" t="n">
         <v>0</v>
@@ -4951,19 +5199,28 @@
       </c>
       <c r="P56" t="inlineStr"/>
       <c r="Q56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R56" t="inlineStr"/>
       <c r="S56" t="inlineStr">
         <is>
-          <t>exponential random agent, rate = 0.1</t>
+          <t>exponential random agent, rate = 0.2</t>
         </is>
       </c>
       <c r="T56" t="inlineStr"/>
-      <c r="U56" t="inlineStr"/>
-      <c r="V56" t="inlineStr"/>
-      <c r="W56" t="inlineStr"/>
-      <c r="X56" t="inlineStr"/>
+      <c r="U56" t="n">
+        <v>187</v>
+      </c>
+      <c r="V56" t="n">
+        <v>250</v>
+      </c>
+      <c r="W56" t="n">
+        <v>143.5000164270401</v>
+      </c>
+      <c r="X56" t="n">
+        <v>2870.000328540802</v>
+      </c>
+      <c r="Y56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -4987,23 +5244,19 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>inversion</t>
+        </is>
+      </c>
+      <c r="G57" t="n">
+        <v>0.2</v>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="I57" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>elitism</t>
+        </is>
+      </c>
+      <c r="I57" t="n">
+        <v>2</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -5019,7 +5272,7 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="N57" t="n">
         <v>0</v>
@@ -5029,19 +5282,28 @@
       </c>
       <c r="P57" t="inlineStr"/>
       <c r="Q57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R57" t="inlineStr"/>
       <c r="S57" t="inlineStr">
         <is>
-          <t>exponential random agent, rate = 0.2</t>
+          <t>exponential random agent, rate = 0.5</t>
         </is>
       </c>
       <c r="T57" t="inlineStr"/>
-      <c r="U57" t="inlineStr"/>
-      <c r="V57" t="inlineStr"/>
-      <c r="W57" t="inlineStr"/>
-      <c r="X57" t="inlineStr"/>
+      <c r="U57" t="n">
+        <v>108</v>
+      </c>
+      <c r="V57" t="n">
+        <v>250</v>
+      </c>
+      <c r="W57" t="n">
+        <v>299.4873049855232</v>
+      </c>
+      <c r="X57" t="n">
+        <v>5989.746099710464</v>
+      </c>
+      <c r="Y57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -5065,23 +5327,19 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>inversion</t>
+        </is>
+      </c>
+      <c r="G58" t="n">
+        <v>0.2</v>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="I58" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>elitism</t>
+        </is>
+      </c>
+      <c r="I58" t="n">
+        <v>2</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -5093,11 +5351,11 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>exponential</t>
+          <t>gaussian</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="N58" t="n">
         <v>0</v>
@@ -5107,19 +5365,28 @@
       </c>
       <c r="P58" t="inlineStr"/>
       <c r="Q58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R58" t="inlineStr"/>
       <c r="S58" t="inlineStr">
         <is>
-          <t>exponential random agent, rate = 0.5</t>
+          <t>gaussian random agent, rate = 0.1</t>
         </is>
       </c>
       <c r="T58" t="inlineStr"/>
-      <c r="U58" t="inlineStr"/>
-      <c r="V58" t="inlineStr"/>
-      <c r="W58" t="inlineStr"/>
-      <c r="X58" t="inlineStr"/>
+      <c r="U58" t="n">
+        <v>170</v>
+      </c>
+      <c r="V58" t="n">
+        <v>250</v>
+      </c>
+      <c r="W58" t="n">
+        <v>156.7604753494263</v>
+      </c>
+      <c r="X58" t="n">
+        <v>3135.209506988525</v>
+      </c>
+      <c r="Y58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -5143,23 +5410,19 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>inversion</t>
+        </is>
+      </c>
+      <c r="G59" t="n">
+        <v>0.2</v>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="I59" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>elitism</t>
+        </is>
+      </c>
+      <c r="I59" t="n">
+        <v>2</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -5175,7 +5438,7 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="N59" t="n">
         <v>0</v>
@@ -5185,19 +5448,28 @@
       </c>
       <c r="P59" t="inlineStr"/>
       <c r="Q59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R59" t="inlineStr"/>
       <c r="S59" t="inlineStr">
         <is>
-          <t>gaussian random agent, rate = 0.1</t>
+          <t>gaussian random agent, rate = 0.2</t>
         </is>
       </c>
       <c r="T59" t="inlineStr"/>
-      <c r="U59" t="inlineStr"/>
-      <c r="V59" t="inlineStr"/>
-      <c r="W59" t="inlineStr"/>
-      <c r="X59" t="inlineStr"/>
+      <c r="U59" t="n">
+        <v>118</v>
+      </c>
+      <c r="V59" t="n">
+        <v>250</v>
+      </c>
+      <c r="W59" t="n">
+        <v>105.6835947275162</v>
+      </c>
+      <c r="X59" t="n">
+        <v>2113.671894550323</v>
+      </c>
+      <c r="Y59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -5221,23 +5493,19 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>inversion</t>
+        </is>
+      </c>
+      <c r="G60" t="n">
+        <v>0.2</v>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="I60" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>elitism</t>
+        </is>
+      </c>
+      <c r="I60" t="n">
+        <v>2</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -5253,7 +5521,7 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="N60" t="n">
         <v>0</v>
@@ -5268,7 +5536,7 @@
       <c r="R60" t="inlineStr"/>
       <c r="S60" t="inlineStr">
         <is>
-          <t>gaussian random agent, rate = 0.2</t>
+          <t>gaussian random agent, rate = 0.5</t>
         </is>
       </c>
       <c r="T60" t="inlineStr"/>
@@ -5276,6 +5544,7 @@
       <c r="V60" t="inlineStr"/>
       <c r="W60" t="inlineStr"/>
       <c r="X60" t="inlineStr"/>
+      <c r="Y60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -5299,23 +5568,19 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>inversion</t>
+        </is>
+      </c>
+      <c r="G61" t="n">
+        <v>0.2</v>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="I61" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>elitism</t>
+        </is>
+      </c>
+      <c r="I61" t="n">
+        <v>2</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -5327,14 +5592,14 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>gaussian</t>
+          <t>None</t>
         </is>
       </c>
       <c r="M61" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="N61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O61" t="n">
         <v>0</v>
@@ -5346,7 +5611,7 @@
       <c r="R61" t="inlineStr"/>
       <c r="S61" t="inlineStr">
         <is>
-          <t>gaussian random agent, rate = 0.5</t>
+          <t>Fitness sharing enabled</t>
         </is>
       </c>
       <c r="T61" t="inlineStr"/>
@@ -5354,6 +5619,7 @@
       <c r="V61" t="inlineStr"/>
       <c r="W61" t="inlineStr"/>
       <c r="X61" t="inlineStr"/>
+      <c r="Y61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -5377,23 +5643,19 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>inversion</t>
+        </is>
+      </c>
+      <c r="G62" t="n">
+        <v>0.2</v>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="I62" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
+          <t>elitism</t>
+        </is>
+      </c>
+      <c r="I62" t="n">
+        <v>2</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -5405,117 +5667,42 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>BEST OF ABOVE</t>
-        </is>
-      </c>
-      <c r="M62" t="inlineStr">
-        <is>
-          <t>BEST OF ABOVE</t>
-        </is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M62" t="n">
+        <v>0</v>
       </c>
       <c r="N62" t="n">
+        <v>0</v>
+      </c>
+      <c r="O62" t="n">
         <v>1</v>
-      </c>
-      <c r="O62" t="n">
-        <v>0</v>
       </c>
       <c r="P62" t="inlineStr"/>
       <c r="Q62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R62" t="inlineStr"/>
       <c r="S62" t="inlineStr">
         <is>
-          <t>Fitness sharing enabled</t>
+          <t>Sparse Reward enabled</t>
         </is>
       </c>
       <c r="T62" t="inlineStr"/>
-      <c r="U62" t="inlineStr"/>
-      <c r="V62" t="inlineStr"/>
-      <c r="W62" t="inlineStr"/>
-      <c r="X62" t="inlineStr"/>
-    </row>
-    <row r="63">
-      <c r="A63" t="n">
-        <v>61</v>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>CartPole-v1</t>
-        </is>
-      </c>
-      <c r="C63" t="n">
-        <v>20</v>
-      </c>
-      <c r="D63" t="n">
-        <v>20</v>
-      </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>4,2</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="H63" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="J63" t="inlineStr">
-        <is>
-          <t>crossover_uniformsplit</t>
-        </is>
-      </c>
-      <c r="K63" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L63" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="M63" t="inlineStr">
-        <is>
-          <t>""</t>
-        </is>
-      </c>
-      <c r="N63" t="inlineStr">
-        <is>
-          <t>BEST OF ABOVE</t>
-        </is>
-      </c>
-      <c r="O63" t="n">
-        <v>1</v>
-      </c>
-      <c r="P63" t="inlineStr"/>
-      <c r="Q63" t="n">
-        <v>0</v>
-      </c>
-      <c r="R63" t="inlineStr"/>
-      <c r="S63" t="inlineStr">
-        <is>
-          <t>Sparse Reward enabled</t>
-        </is>
-      </c>
-      <c r="T63" t="inlineStr"/>
-      <c r="U63" t="inlineStr"/>
-      <c r="V63" t="inlineStr"/>
-      <c r="W63" t="inlineStr"/>
-      <c r="X63" t="inlineStr"/>
+      <c r="U62" t="n">
+        <v>165</v>
+      </c>
+      <c r="V62" t="n">
+        <v>1035</v>
+      </c>
+      <c r="W62" t="n">
+        <v>2.163300538063049</v>
+      </c>
+      <c r="X62" t="n">
+        <v>43.26601076126099</v>
+      </c>
+      <c r="Y62" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>